<commit_message>
docs: update normalisasi, probably will update it by using an api
</commit_message>
<xml_diff>
--- a/data/reference/normalisasi.xlsx
+++ b/data/reference/normalisasi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\procurement-processor\data\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178AD5F3-3F1B-44ED-93F5-98ACC4AD0825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2789205C-54E7-4FD9-83C4-D3F29CD4D0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="206">
   <si>
     <t>Requisition Number</t>
   </si>
@@ -654,6 +654,12 @@
   </si>
   <si>
     <t xml:space="preserve">pec lama seperi di rfm sudah tidak ada sehingga pakai spec persamaan </t>
+  </si>
+  <si>
+    <t>6097-20482</t>
+  </si>
+  <si>
+    <t>BAST baru dapat dari user</t>
   </si>
 </sst>
 </file>
@@ -892,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2414,6 +2420,20 @@
         <v>100</v>
       </c>
     </row>
+    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="3">
+        <v>45982</v>
+      </c>
+      <c r="D103" t="s">
+        <v>205</v>
+      </c>
+      <c r="F103" t="s">
+        <v>186</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D99" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2423,11 +2443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3685549-0E80-4F97-95AA-FF34889F39A4}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:B108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2441,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2450,7 +2469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2459,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2468,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2477,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2486,7 +2505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2495,7 +2514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2504,7 +2523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2513,7 +2532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2522,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2531,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2540,7 +2559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2549,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2558,7 +2577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2567,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2576,7 +2595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2585,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2594,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
@@ -2603,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2612,7 +2631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2621,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -2630,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2639,7 +2658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2648,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -2657,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -2666,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2675,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -2684,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2693,7 +2712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -2702,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2711,7 +2730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -2720,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -2729,7 +2748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2738,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2747,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2756,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -2765,7 +2784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -2774,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -2783,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -2792,7 +2811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -2801,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -2810,7 +2829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -2819,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -2828,7 +2847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -2837,7 +2856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -2846,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -2855,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2864,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -2873,7 +2892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -2882,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -2891,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -2900,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>108</v>
       </c>
@@ -2909,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>110</v>
       </c>
@@ -2918,7 +2937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -2927,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -2936,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>115</v>
       </c>
@@ -2945,7 +2964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>118</v>
       </c>
@@ -2954,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>121</v>
       </c>
@@ -2963,7 +2982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>122</v>
       </c>
@@ -2972,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>123</v>
       </c>
@@ -2981,7 +3000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>124</v>
       </c>
@@ -2990,7 +3009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -2999,7 +3018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>107</v>
       </c>
@@ -3008,7 +3027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>120</v>
       </c>
@@ -3017,7 +3036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>130</v>
       </c>
@@ -3026,7 +3045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>132</v>
       </c>
@@ -3035,7 +3054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>134</v>
       </c>
@@ -3044,7 +3063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>135</v>
       </c>
@@ -3053,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>137</v>
       </c>
@@ -3062,7 +3081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -3071,7 +3090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>139</v>
       </c>
@@ -3080,7 +3099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>140</v>
       </c>
@@ -3098,7 +3117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>142</v>
       </c>
@@ -3107,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>143</v>
       </c>
@@ -3116,7 +3135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -3125,7 +3144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>147</v>
       </c>
@@ -3134,7 +3153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>149</v>
       </c>
@@ -3143,7 +3162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>159</v>
       </c>
@@ -3152,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>161</v>
       </c>
@@ -3161,7 +3180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -3170,7 +3189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>164</v>
       </c>
@@ -3179,7 +3198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>137</v>
       </c>
@@ -3188,7 +3207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>139</v>
       </c>
@@ -3197,7 +3216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>138</v>
       </c>
@@ -3206,7 +3225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>168</v>
       </c>
@@ -3215,7 +3234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>170</v>
       </c>
@@ -3224,7 +3243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>149</v>
       </c>
@@ -3233,7 +3252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>173</v>
       </c>
@@ -3242,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>147</v>
       </c>
@@ -3251,7 +3270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>175</v>
       </c>
@@ -3260,7 +3279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>177</v>
       </c>
@@ -3269,7 +3288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>178</v>
       </c>
@@ -3278,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>179</v>
       </c>
@@ -3287,7 +3306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>180</v>
       </c>
@@ -3296,7 +3315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>181</v>
       </c>
@@ -3314,7 +3333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>182</v>
       </c>
@@ -3323,7 +3342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>140</v>
       </c>
@@ -3332,7 +3351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>184</v>
       </c>
@@ -3341,7 +3360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>187</v>
       </c>
@@ -3350,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>190</v>
       </c>
@@ -3359,7 +3378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -3386,7 +3405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>196</v>
       </c>
@@ -3395,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>198</v>
       </c>
@@ -3405,13 +3424,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B108" xr:uid="{C3685549-0E80-4F97-95AA-FF34889F39A4}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="4"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:B108" xr:uid="{C3685549-0E80-4F97-95AA-FF34889F39A4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>